<commit_message>
A little cleen up
</commit_message>
<xml_diff>
--- a/Images-Need_translation/Worksheet.xlsx
+++ b/Images-Need_translation/Worksheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="313">
   <si>
     <t>毎回</t>
   </si>
@@ -489,12 +489,561 @@
       <t xml:space="preserve"> gallery</t>
     </r>
   </si>
+  <si>
+    <t>AMScratch</t>
+  </si>
+  <si>
+    <t>AM運動カードGold</t>
+  </si>
+  <si>
+    <t>AM Exercise Card Gold</t>
+  </si>
+  <si>
+    <t>AM_Card_Gold.png</t>
+  </si>
+  <si>
+    <t>AM運動カード</t>
+  </si>
+  <si>
+    <t>AM Exercise Card</t>
+  </si>
+  <si>
+    <t>AM_Card_Normal.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AM運動カードPlatinum </t>
+  </si>
+  <si>
+    <t>AM Exercise Card Platinum</t>
+  </si>
+  <si>
+    <t>AM_Card_Platinum.png</t>
+  </si>
+  <si>
+    <t>AM運動カードPremium</t>
+  </si>
+  <si>
+    <t>AM Exercise Card Premium</t>
+  </si>
+  <si>
+    <t>AM_Card_Premium.png</t>
+  </si>
+  <si>
+    <t>AM Exercise Card Silver</t>
+  </si>
+  <si>
+    <t>AM運動カードSilver</t>
+  </si>
+  <si>
+    <t>AM_Card_Silver.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/CameraSetting/CamSet_Tit02a.png</t>
+  </si>
+  <si>
+    <t>交換パーツ効果 - Effect of spare part</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/CameraSetting/CamSet_Tit03.png</t>
+  </si>
+  <si>
+    <t>記録カード - Memory card</t>
+  </si>
+  <si>
+    <t>レンズ - Lens</t>
+  </si>
+  <si>
+    <t>手ぶれ補正 - Image stabilisation</t>
+  </si>
+  <si>
+    <t>特殊効果 - Special effects</t>
+  </si>
+  <si>
+    <t>交換パーツ - Spare part</t>
+  </si>
+  <si>
+    <t>CameraSetting</t>
+  </si>
+  <si>
+    <t>CamSet_Alert00.png</t>
+  </si>
+  <si>
+    <t>撮影モード中はパーツの交換はできません。</t>
+  </si>
+  <si>
+    <t>Unable to change spare part while in Shooting Mode.</t>
+  </si>
+  <si>
+    <t>CamSet_Alert01.png</t>
+  </si>
+  <si>
+    <t>撮影モード中でも特殊効果を変更することができません。</t>
+  </si>
+  <si>
+    <t>Unable to change special effects while in Shooting Mode</t>
+  </si>
+  <si>
+    <t>CamSet_Info_00.png</t>
+  </si>
+  <si>
+    <t>なし</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Camera_Btn01/Btn_kamae_a.png</t>
+  </si>
+  <si>
+    <t>カメラ - Camera</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Camera_Btn01/Btn_kamae_b.bclim</t>
+  </si>
+  <si>
+    <t>(image not extracted)</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/ShopPanel01_text01.png</t>
+  </si>
+  <si>
+    <t>記録カードを購入すると以前の撮影枚数には戻せません。 - Upon buying a new memory card, you will be unable to revert to the previous capacity.</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_Pnl4_category01.png</t>
+  </si>
+  <si>
+    <t>アクセサリー - Accessories</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_Pnl4_category02.png</t>
+  </si>
+  <si>
+    <t>衣服 - Clothing</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_Pnl4_category03.png</t>
+  </si>
+  <si>
+    <t>食器 - Tableware</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_Pnl4_category04.png</t>
+  </si>
+  <si>
+    <t>コスプレアイテム - Cosplay items</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_Pnl4_category07.png</t>
+  </si>
+  <si>
+    <t>カメラ - Camera goods</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_Pnl4_category08.png</t>
+  </si>
+  <si>
+    <t>本 - Books</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_Pnl4_category09.png</t>
+  </si>
+  <si>
+    <t>食べ物 - Food</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_Pnl4_category10.png</t>
+  </si>
+  <si>
+    <t>小物 - Trinkets</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_RichTxt01.png</t>
+  </si>
+  <si>
+    <t>リッチ - Rich</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_RichTxt02.png</t>
+  </si>
+  <si>
+    <t>所持リッチ： - Rich on hand:</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_RichTxt03.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_TitTxt00.png</t>
+  </si>
+  <si>
+    <t>商品一覧 - All items</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Shop/Shop_TitTxt04.png</t>
+  </si>
+  <si>
+    <t>MeetingTime/Meet_Day_01 to 07</t>
+  </si>
+  <si>
+    <t>In order:</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>[22:57]</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/FileSelect/timg/D_Select_txt01.png</t>
+  </si>
+  <si>
+    <t>データを選択して下さい - Please select data</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/FileSelect/timg/D_Select_data01.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/FileSelect/timg/D_Select_data02.png</t>
+  </si>
+  <si>
+    <t>データを選択して下さい - Please Select Data</t>
+  </si>
+  <si>
+    <t>データ更新 - Data Update</t>
+  </si>
+  <si>
+    <t>名前 - Name</t>
+  </si>
+  <si>
+    <t>呼ばれ方 - Nickname</t>
+  </si>
+  <si>
+    <t>H N - Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">誕生日 - Birthday </t>
+  </si>
+  <si>
+    <t>血液型 - Blood Type</t>
+  </si>
+  <si>
+    <t>出身地 - Birthplace</t>
+  </si>
+  <si>
+    <t>経過日数 - Days Passed</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/FileSelect/timg/D_Select_data03.png</t>
+  </si>
+  <si>
+    <t>交際期間 - Dating Period</t>
+  </si>
+  <si>
+    <t>称号 - Title</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt01.png</t>
+  </si>
+  <si>
+    <t>名前 - Family Name</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt02.png</t>
+  </si>
+  <si>
+    <t>呼ばれ方 - First Name</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt03.png</t>
+  </si>
+  <si>
+    <t>誕生日 - Birthday</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt04.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt05.png</t>
+  </si>
+  <si>
+    <t>出身 - Birthplace</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt06.png</t>
+  </si>
+  <si>
+    <t>カノジョの名前 - Girlfriend's Name</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt07.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt08.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card04_txt09.png</t>
+  </si>
+  <si>
+    <t>ミニゲーム - Minigames</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/Bc_04_b_btn1_lite.png</t>
+  </si>
+  <si>
+    <t>本名　HN - Real Name     Username</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/Flist_Name01.png</t>
+  </si>
+  <si>
+    <t>友だちリストあああ - Friend List AAA</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/Flist_Txt01.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/Flist_Txt02.png</t>
+  </si>
+  <si>
+    <t>フレンド/ロック - Friend/Block</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/Flist_Txt03.png</t>
+  </si>
+  <si>
+    <t>受信日時 - Received Date</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Card/B_Card_SealCount_Base.png</t>
+  </si>
+  <si>
+    <t>残り枚数 - Pages Remaining</t>
+  </si>
+  <si>
+    <t>Card/B_Card_SealCount_Base_A01 to 06</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/CmdJudge/AcInfo_01_Mess00.png</t>
+  </si>
+  <si>
+    <t>ダミーテキスト - Dummy Text</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/CmdJudge/AcInfo_02_MessPre02.png</t>
+  </si>
+  <si>
+    <t>カノジョから - From Girlfriend</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/CmdJudge/AcInfo_02_MessSuf01.png</t>
+  </si>
+  <si>
+    <t>電話 - Phone</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/CmdJudge/AcInfo_02_MessSuf02.png</t>
+  </si>
+  <si>
+    <t>メール - E-Mail</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/CmdJudge/AcInfo_02_Time01.png</t>
+  </si>
+  <si>
+    <t>予定 - Schedule</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/CmdJudge/Tel_rest1.png</t>
+  </si>
+  <si>
+    <t>残り時間 - Time Remaining</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Camera_Pv03/Camera_Pv03.png</t>
+  </si>
+  <si>
+    <t>セーブ中 - Saving</t>
+  </si>
+  <si>
+    <t>https://github.com/Makein/NLPPGit/blob/master/Images-Need_translation/Camera_Btn04/Btn_Large_R_a.png</t>
+  </si>
+  <si>
+    <t>撮影する - Take Photo</t>
+  </si>
+  <si>
+    <t>Camera_Btn04/Btn_Large_R_b and c</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>Camera_Btn03/Filter_Txt00 to 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">カメラフィルターなし - No Filter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ソフトフォーカス大 - High Soft Focus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ソフトフォーカス小 - Low Soft Focus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">被写界深度強調大 - High Depth of Field Enhancement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">被写界深度強調小 - Low Depth of Field Enhancement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDR強調大 - High HDR Increase </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDR強調小 - Low HDR Increase </t>
+  </si>
+  <si>
+    <t xml:space="preserve">トイカメラ：明るい緑 - Toy Camera : Bright Green </t>
+  </si>
+  <si>
+    <t xml:space="preserve">トイカメラ：暗い緑 - Toy Camera : Dark Green </t>
+  </si>
+  <si>
+    <t xml:space="preserve">トイカメラ：明るい黄色 - Toy Camera : Bright Yellow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">トイカメラ：暗い黄色 - Toy Camera : Dark Yellow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">インスタントカメラ：標準 - Instant Camera : Standard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">インスタントカメラ：黄み強調 - Instant Camera : Increased Yellow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">インスタントカメラ：青み強調 - Instant Camera : Increased Blue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">インスタントカメラ：赤み強調 - Instant Camera : Increased Red </t>
+  </si>
+  <si>
+    <t xml:space="preserve">アンティーク：明るいセピア - Antique : Bright Sepia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">アンティーク：暗いセピア - Antique : Dark Sepia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">アンティーク：明るい白黒 - Antique : Bright Black and White </t>
+  </si>
+  <si>
+    <t>アンティーク：暗い白黒 - Antique : Dark Black and White</t>
+  </si>
+  <si>
+    <t>CamSet_Info_01.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">視線軽減・消音 </t>
+  </si>
+  <si>
+    <t>Line of sight reduced/Silenced</t>
+  </si>
+  <si>
+    <t>CamSet_Info_02.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">視線軽減 </t>
+  </si>
+  <si>
+    <t>Line of sight reduced</t>
+  </si>
+  <si>
+    <t>CamSet_Info_03.png</t>
+  </si>
+  <si>
+    <t>CamSet_Info_04.png</t>
+  </si>
+  <si>
+    <t>CamSet_Info_05.png</t>
+  </si>
+  <si>
+    <t>CamSet_Text01.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">緊張アップ </t>
+  </si>
+  <si>
+    <t>Nervousness Up</t>
+  </si>
+  <si>
+    <t>Relax</t>
+  </si>
+  <si>
+    <t>Temporary Mood Up</t>
+  </si>
+  <si>
+    <t>一時ムードアップ</t>
+  </si>
+  <si>
+    <t>リラックス</t>
+  </si>
+  <si>
+    <t xml:space="preserve">撮影枚数　少 ... 多(　枚) </t>
+  </si>
+  <si>
+    <t>Number of photos  Less...More ( sheets)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ズーム　小 ...　大 (x　) </t>
+  </si>
+  <si>
+    <t>Zoom  Small...Large (x )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">手ぶれ補正　弱 ...　強 </t>
+  </si>
+  <si>
+    <t>Image stabilisation  Weak...Strong</t>
+  </si>
+  <si>
+    <t>ステルス　小 ...　大</t>
+  </si>
+  <si>
+    <t>Stealth  Slight...Large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">シャッター音　小 ...　大 </t>
+  </si>
+  <si>
+    <t>Shutter sound  Soft...Loud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ズーム音　小 ...　大 </t>
+  </si>
+  <si>
+    <t>Zoom sound  Soft...Loud</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,12 +1080,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -562,18 +1120,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -902,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1772,7 +2337,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -1780,7 +2345,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -1788,7 +2353,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>84</v>
       </c>
@@ -1796,7 +2361,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -1804,12 +2369,1014 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>84</v>
       </c>
       <c r="B69" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="6"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="6"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1">
+      <c r="A270" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1">
+      <c r="A272" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1">
+      <c r="A276" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1">
+      <c r="A280" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1">
+      <c r="A282" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1">
+      <c r="A284" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1">
+      <c r="A286" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1">
+      <c r="A288" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1">
+      <c r="A290" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1">
+      <c r="A292" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1">
+      <c r="A294" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1">
+      <c r="A296" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1">
+      <c r="A298" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1">
+      <c r="A302" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1">
+      <c r="A304" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1">
+      <c r="A306" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1">
+      <c r="A308" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1">
+      <c r="A310" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1">
+      <c r="A312" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1">
+      <c r="A314" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1">
+      <c r="A316" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1">
+      <c r="A318" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1">
+      <c r="A320" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1">
+      <c r="A322" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1">
+      <c r="A324" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1">
+      <c r="A326" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1">
+      <c r="A328" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1">
+      <c r="A330" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1">
+      <c r="A332" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1">
+      <c r="A334" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1">
+      <c r="A336" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1">
+      <c r="A338" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1">
+      <c r="A340" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1">
+      <c r="A342" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1">
+      <c r="A344" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1">
+      <c r="A346" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1">
+      <c r="A348" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1">
+      <c r="A350" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1">
+      <c r="A352" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1">
+      <c r="A354" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1">
+      <c r="A356" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1">
+      <c r="A358" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1">
+      <c r="A360" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>